<commit_message>
Se crea archivo RMD
</commit_message>
<xml_diff>
--- a/B_D_CAT.xlsx
+++ b/B_D_CAT.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmaureira\Documents\Diplomado R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BC606A-710A-4AA6-891D-C4498AEB6EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383949FE-4ED6-48B1-8A95-C53DB6D9F7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{8D98E46B-50FD-4F95-8510-632B900E3ED4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$3207</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -70,7 +73,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -103,7 +106,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -421,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1137D86-A63D-471B-AA4B-E225A520C7D4}">
   <dimension ref="A1:H3207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A1142" workbookViewId="0">
+      <selection activeCell="G1149" sqref="G1149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -69196,11 +69199,11 @@
         <v>1900</v>
       </c>
       <c r="F3051">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="G3051" s="1">
         <f t="shared" si="47"/>
-        <v>1520</v>
+        <v>1.52</v>
       </c>
       <c r="H3051">
         <v>12</v>
@@ -72819,6 +72822,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H3207" xr:uid="{B1137D86-A63D-471B-AA4B-E225A520C7D4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>